<commit_message>
Pruebas hasta pagos de los cupones
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/Sedes.xlsx
+++ b/MercuryTours/Resources/datapool/Sedes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12900" windowHeight="3945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14025" windowHeight="5070"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Nombre</t>
   </si>
@@ -87,6 +87,27 @@
   </si>
   <si>
     <t>Salento</t>
+  </si>
+  <si>
+    <t>calle 4 #12-17</t>
+  </si>
+  <si>
+    <t>calle 13n #18-34</t>
+  </si>
+  <si>
+    <t>calle 13n #18-35</t>
+  </si>
+  <si>
+    <t>calle 13n #18-36</t>
+  </si>
+  <si>
+    <t>calle 13n #18-37</t>
+  </si>
+  <si>
+    <t>calle 13n #18-38</t>
+  </si>
+  <si>
+    <t>calle 13n #18-39</t>
   </si>
 </sst>
 </file>
@@ -432,7 +453,7 @@
   <dimension ref="A2:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -471,6 +492,15 @@
       </c>
       <c r="J2" t="s">
         <v>5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -490,10 +520,28 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>